<commit_message>
add example terms for GEO templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/GEO/GEO_-_High-throughput_sequencing_-_Assay.xlsx
+++ b/templates/dataplant/GEO/GEO_-_High-throughput_sequencing_-_Assay.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -245,10 +245,22 @@
     <t>user-specific</t>
   </si>
   <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>paired-end</t>
+    <t>libraryconstruction.txt</t>
+  </si>
+  <si>
+    <t>single-end</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/DPBO_0000086</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 2000</t>
+  </si>
+  <si>
+    <t>OBI</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/OBI_0002001</t>
   </si>
 </sst>
 </file>
@@ -304,8 +316,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:R5" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:R5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:R2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:R2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -885,7 +897,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:R2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -958,7 +970,7 @@
         <v>74</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
         <v>74</v>
@@ -970,201 +982,33 @@
         <v>74</v>
       </c>
       <c r="I2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J2" t="s">
-        <v>74</v>
+        <v>19</v>
       </c>
       <c r="K2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="L2" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
       <c r="M2" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="N2" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="O2" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="P2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="Q2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="R2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I3" t="s">
-        <v>78</v>
-      </c>
-      <c r="J3" t="s">
-        <v>74</v>
-      </c>
-      <c r="K3" t="s">
-        <v>74</v>
-      </c>
-      <c r="L3" t="s">
-        <v>74</v>
-      </c>
-      <c r="M3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" t="s">
-        <v>74</v>
-      </c>
-      <c r="O3" t="s">
-        <v>74</v>
-      </c>
-      <c r="P3" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>74</v>
-      </c>
-      <c r="R3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" t="s">
-        <v>74</v>
-      </c>
-      <c r="H4" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" t="s">
-        <v>74</v>
-      </c>
-      <c r="J4" t="s">
-        <v>74</v>
-      </c>
-      <c r="K4" t="s">
-        <v>74</v>
-      </c>
-      <c r="L4" t="s">
-        <v>74</v>
-      </c>
-      <c r="M4" t="s">
-        <v>74</v>
-      </c>
-      <c r="N4" t="s">
-        <v>74</v>
-      </c>
-      <c r="O4" t="s">
-        <v>74</v>
-      </c>
-      <c r="P4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" t="s">
-        <v>74</v>
-      </c>
-      <c r="F5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H5" t="s">
-        <v>74</v>
-      </c>
-      <c r="I5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" t="s">
-        <v>74</v>
-      </c>
-      <c r="K5" t="s">
-        <v>74</v>
-      </c>
-      <c r="L5" t="s">
-        <v>74</v>
-      </c>
-      <c r="M5" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" t="s">
-        <v>74</v>
-      </c>
-      <c r="O5" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>